<commit_message>
added csr module, updated test driving, small rtl fixes
</commit_message>
<xml_diff>
--- a/docs/spreadsheets/instr_decode_table.xlsx
+++ b/docs/spreadsheets/instr_decode_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="132">
   <si>
     <t xml:space="preserve">Mnemonic</t>
   </si>
@@ -64,6 +64,15 @@
     <t xml:space="preserve">width_src</t>
   </si>
   <si>
+    <t xml:space="preserve">csr_we</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csr_src</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csr_control</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
@@ -106,6 +115,9 @@
     <t xml:space="preserve">WIDTH_32</t>
   </si>
   <si>
+    <t xml:space="preserve">NO_WRITE_CSR</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUB</t>
   </si>
   <si>
@@ -367,16 +379,37 @@
     <t xml:space="preserve">CSRRW</t>
   </si>
   <si>
+    <t xml:space="preserve">RESULT_CSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WRITE_CSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSR_SRC_REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSR_PASS</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSRRS</t>
   </si>
   <si>
+    <t xml:space="preserve">CSR_SET</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSRRC</t>
   </si>
   <si>
+    <t xml:space="preserve">CSR_CLEAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSRRWI</t>
   </si>
   <si>
     <t xml:space="preserve">CSR_EXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSR_SRC_IMM</t>
   </si>
   <si>
     <t xml:space="preserve">CSRRSI</t>
@@ -502,27 +535,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39:G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="9.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,1802 +609,2294 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="J16" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="N20" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="O22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="O23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="G28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>75</v>
+      <c r="O28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="L29" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O29" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="G31" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O31" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="I32" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="K33" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O35" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O37" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="O38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>1110011</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q39" s="0" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>1110011</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q40" s="0" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>1110011</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>1110011</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O42" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q42" s="0" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>1110011</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q43" s="0" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>1110011</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O44" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="P44" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q44" s="0" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2"/>

</xml_diff>